<commit_message>
City index 25-10 update 4/12.
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_16952.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_16952.xlsx
@@ -2663,15 +2663,6 @@
       <c r="D4">
         <v>2025</v>
       </c>
-      <c r="F4">
-        <v>4.73</v>
-      </c>
-      <c r="G4">
-        <v>12.64</v>
-      </c>
-      <c r="H4">
-        <v>-8.69</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2987,6 +2978,9 @@
       <c r="M13">
         <v>5.6</v>
       </c>
+      <c r="N13">
+        <v>1.78</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3146,6 +3140,9 @@
       <c r="M16">
         <v>3.66</v>
       </c>
+      <c r="N16">
+        <v>3.49</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3305,6 +3302,9 @@
       <c r="M19">
         <v>-0.87</v>
       </c>
+      <c r="N19">
+        <v>5.67</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3590,6 +3590,9 @@
       <c r="M25">
         <v>-2.61</v>
       </c>
+      <c r="N25">
+        <v>-2.89</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3968,6 +3971,9 @@
       <c r="M34">
         <v>4.69</v>
       </c>
+      <c r="N34">
+        <v>5.88</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4250,6 +4256,9 @@
       <c r="M40">
         <v>3.26</v>
       </c>
+      <c r="N40">
+        <v>2.24</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4664,6 +4673,9 @@
       <c r="M49">
         <v>5.07</v>
       </c>
+      <c r="N49">
+        <v>2.43</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4928,18 +4940,6 @@
       <c r="D55">
         <v>2025</v>
       </c>
-      <c r="E55">
-        <v>0.27</v>
-      </c>
-      <c r="F55">
-        <v>0.92</v>
-      </c>
-      <c r="I55">
-        <v>-7.01</v>
-      </c>
-      <c r="K55">
-        <v>2.41</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -5099,6 +5099,9 @@
       <c r="M58">
         <v>-3.25</v>
       </c>
+      <c r="N58">
+        <v>-4.11</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5258,6 +5261,9 @@
       <c r="M61">
         <v>0.96</v>
       </c>
+      <c r="N61">
+        <v>7.25</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5411,6 +5417,9 @@
       <c r="M64">
         <v>4.34</v>
       </c>
+      <c r="N64">
+        <v>2.87</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5720,6 +5729,9 @@
       <c r="M73">
         <v>0.22</v>
       </c>
+      <c r="N73">
+        <v>-0.33</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -5846,6 +5858,9 @@
       <c r="M76">
         <v>9.390000000000001</v>
       </c>
+      <c r="N76">
+        <v>9.93</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -5972,6 +5987,9 @@
       <c r="M79">
         <v>10.64</v>
       </c>
+      <c r="N79">
+        <v>8.1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -6103,9 +6121,6 @@
       </c>
       <c r="F82">
         <v>4.86</v>
-      </c>
-      <c r="K82">
-        <v>-2.92</v>
       </c>
     </row>
   </sheetData>
@@ -6272,7 +6287,7 @@
         <v>-6.2</v>
       </c>
       <c r="J3">
-        <v>1.187051640246083</v>
+        <v>1.18240265755164</v>
       </c>
       <c r="K3">
         <v>-8.5</v>
@@ -6321,7 +6336,7 @@
         <v>4.3</v>
       </c>
       <c r="J4">
-        <v>2.080944899441648</v>
+        <v>2.077955497173004</v>
       </c>
       <c r="K4">
         <v>0.2</v>
@@ -6343,7 +6358,7 @@
         <v>2025</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6357,26 +6372,26 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>jan-sep</t>
+          <t>jan-okt</t>
         </is>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5">
-        <v>1.0117</v>
+        <v>1.014</v>
       </c>
       <c r="I5">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="J5">
-        <v>1.004318564843871</v>
+        <v>1.116766126251205</v>
       </c>
       <c r="K5">
         <v>-0.8</v>
       </c>
       <c r="L5">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -6419,7 +6434,7 @@
         <v>-2.2</v>
       </c>
       <c r="J6">
-        <v>2.31131451621699</v>
+        <v>2.306349631338904</v>
       </c>
       <c r="K6">
         <v>-6.7</v>
@@ -6465,7 +6480,7 @@
         <v>-10.15876000000001</v>
       </c>
       <c r="J7">
-        <v>1.400933741259997</v>
+        <v>1.397320590274238</v>
       </c>
       <c r="K7">
         <v>-12.9</v>
@@ -6511,7 +6526,7 @@
         <v>-6.28660255600002</v>
       </c>
       <c r="J8">
-        <v>2.373076760327225</v>
+        <v>2.368639008242137</v>
       </c>
       <c r="K8">
         <v>-10.9</v>
@@ -6532,7 +6547,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7600,55 +7615,55 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>0.9407166855002579</v>
+        <v>0.9568554091875735</v>
       </c>
       <c r="B24">
-        <v>-5.928331449974211</v>
+        <v>-4.314459081242649</v>
       </c>
       <c r="C24">
         <v>14</v>
       </c>
       <c r="D24">
-        <v>9.85146347193337</v>
+        <v>9.461194469994499</v>
       </c>
       <c r="E24">
-        <v>7.329273390694706</v>
+        <v>10.62561012946104</v>
       </c>
       <c r="F24">
-        <v>2.395542921504799</v>
+        <v>3.422293990449863</v>
       </c>
       <c r="G24">
-        <v>-10.6</v>
+        <v>-11</v>
       </c>
       <c r="H24">
-        <v>-1.2</v>
+        <v>2.4</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2019 - (jan 2023 - des 2024)</t>
+          <t>2019 - (nov 2024 - okt 2025)</t>
         </is>
       </c>
       <c r="J24" s="2">
-        <v>45627</v>
+        <v>45931</v>
       </c>
       <c r="K24">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L24">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>24_months</t>
+          <t>12_months</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>0.9448885225160316</v>
+        <v>0.9407166855002579</v>
       </c>
       <c r="B25">
-        <v>-5.511147748396839</v>
+        <v>-5.928331449974211</v>
       </c>
       <c r="C25">
         <v>14</v>
@@ -7657,30 +7672,30 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E25">
-        <v>7.751253966998971</v>
+        <v>7.329273390694706</v>
       </c>
       <c r="F25">
-        <v>2.5175465032293</v>
+        <v>2.395542921504799</v>
       </c>
       <c r="G25">
-        <v>-10.4</v>
+        <v>-10.6</v>
       </c>
       <c r="H25">
-        <v>-0.6</v>
+        <v>-1.2</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2019 - (feb 2023 - jan 2025)</t>
+          <t>2019 - (jan 2023 - des 2024)</t>
         </is>
       </c>
       <c r="J25" s="2">
-        <v>45658</v>
+        <v>45627</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L25">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
@@ -7690,10 +7705,10 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>0.9493633079377803</v>
+        <v>0.9448885225160316</v>
       </c>
       <c r="B26">
-        <v>-5.063669206221966</v>
+        <v>-5.511147748396839</v>
       </c>
       <c r="C26">
         <v>14</v>
@@ -7702,27 +7717,27 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E26">
-        <v>8.199525507506396</v>
+        <v>7.751253966998971</v>
       </c>
       <c r="F26">
-        <v>2.647875692112421</v>
+        <v>2.5175465032293</v>
       </c>
       <c r="G26">
-        <v>-10.3</v>
+        <v>-10.4</v>
       </c>
       <c r="H26">
-        <v>0.1</v>
+        <v>-0.6</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2019 - (mar 2023 - feb 2025)</t>
+          <t>2019 - (feb 2023 - jan 2025)</t>
         </is>
       </c>
       <c r="J26" s="2">
-        <v>45689</v>
+        <v>45658</v>
       </c>
       <c r="K26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L26">
         <v>2025</v>
@@ -7735,10 +7750,10 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>0.9501717700140583</v>
+        <v>0.9493633079377803</v>
       </c>
       <c r="B27">
-        <v>-4.982822998594171</v>
+        <v>-5.063669206221966</v>
       </c>
       <c r="C27">
         <v>14</v>
@@ -7747,27 +7762,27 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E27">
-        <v>8.616161112309243</v>
+        <v>8.199525507506396</v>
       </c>
       <c r="F27">
-        <v>2.768619629046594</v>
+        <v>2.647875692112421</v>
       </c>
       <c r="G27">
-        <v>-10.4</v>
+        <v>-10.3</v>
       </c>
       <c r="H27">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2019 - (apr 2023 - mar 2025)</t>
+          <t>2019 - (mar 2023 - feb 2025)</t>
         </is>
       </c>
       <c r="J27" s="2">
-        <v>45717</v>
+        <v>45689</v>
       </c>
       <c r="K27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L27">
         <v>2025</v>
@@ -7780,10 +7795,10 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>0.9538765915536376</v>
+        <v>0.9501717700140583</v>
       </c>
       <c r="B28">
-        <v>-4.612340844636242</v>
+        <v>-4.982822998594171</v>
       </c>
       <c r="C28">
         <v>14</v>
@@ -7792,27 +7807,27 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E28">
-        <v>9.190469092064667</v>
+        <v>8.616161112309243</v>
       </c>
       <c r="F28">
-        <v>2.936645120593631</v>
+        <v>2.768619629046594</v>
       </c>
       <c r="G28">
         <v>-10.4</v>
       </c>
       <c r="H28">
-        <v>1.1</v>
+        <v>0.4</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2019 - (mai 2023 - apr 2025)</t>
+          <t>2019 - (apr 2023 - mar 2025)</t>
         </is>
       </c>
       <c r="J28" s="2">
-        <v>45748</v>
+        <v>45717</v>
       </c>
       <c r="K28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L28">
         <v>2025</v>
@@ -7825,10 +7840,10 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>0.9566542182687537</v>
+        <v>0.9538765915536376</v>
       </c>
       <c r="B29">
-        <v>-4.334578173124626</v>
+        <v>-4.612340844636242</v>
       </c>
       <c r="C29">
         <v>14</v>
@@ -7837,27 +7852,27 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E29">
-        <v>9.660527652721862</v>
+        <v>9.190469092064667</v>
       </c>
       <c r="F29">
-        <v>3.074711764079583</v>
+        <v>2.936645120593631</v>
       </c>
       <c r="G29">
         <v>-10.4</v>
       </c>
       <c r="H29">
-        <v>1.7</v>
+        <v>1.1</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2019 - (jun 2023 - mai 2025)</t>
+          <t>2019 - (mai 2023 - apr 2025)</t>
         </is>
       </c>
       <c r="J29" s="2">
-        <v>45778</v>
+        <v>45748</v>
       </c>
       <c r="K29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L29">
         <v>2025</v>
@@ -7870,39 +7885,39 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>0.9337995597988019</v>
+        <v>0.9566542182687537</v>
       </c>
       <c r="B30">
-        <v>-6.620044020119808</v>
+        <v>-4.334578173124626</v>
       </c>
       <c r="C30">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D30">
-        <v>8.176539225649242</v>
+        <v>9.85146347193337</v>
       </c>
       <c r="E30">
-        <v>7.9106263041602</v>
+        <v>9.660527652721862</v>
       </c>
       <c r="F30">
-        <v>2.783454672675907</v>
+        <v>3.074711764079583</v>
       </c>
       <c r="G30">
-        <v>-12.1</v>
+        <v>-10.4</v>
       </c>
       <c r="H30">
-        <v>-1.2</v>
+        <v>1.7</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2019 - (jul 2023 - jun 2025)</t>
+          <t>2019 - (jun 2023 - mai 2025)</t>
         </is>
       </c>
       <c r="J30" s="2">
-        <v>45809</v>
+        <v>45778</v>
       </c>
       <c r="K30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L30">
         <v>2025</v>
@@ -7915,39 +7930,39 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>0.9355678479216543</v>
+        <v>0.9337995597988019</v>
       </c>
       <c r="B31">
-        <v>-6.443215207834574</v>
+        <v>-6.620044020119808</v>
       </c>
       <c r="C31">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D31">
-        <v>7.442799395296631</v>
+        <v>8.176539225649242</v>
       </c>
       <c r="E31">
-        <v>8.880892518164108</v>
+        <v>7.9106263041602</v>
       </c>
       <c r="F31">
-        <v>3.232957748931967</v>
+        <v>2.783454672675907</v>
       </c>
       <c r="G31">
-        <v>-12.8</v>
+        <v>-12.1</v>
       </c>
       <c r="H31">
-        <v>-0.1</v>
+        <v>-1.2</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2019 - (aug 2023 - jul 2025)</t>
+          <t>2019 - (jul 2023 - jun 2025)</t>
         </is>
       </c>
       <c r="J31" s="2">
-        <v>45839</v>
+        <v>45809</v>
       </c>
       <c r="K31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L31">
         <v>2025</v>
@@ -7960,39 +7975,39 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>0.9424201687562938</v>
+        <v>0.9355678479216543</v>
       </c>
       <c r="B32">
-        <v>-5.757983124370625</v>
+        <v>-6.443215207834574</v>
       </c>
       <c r="C32">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>8.761728922821021</v>
+        <v>7.442799395296631</v>
       </c>
       <c r="E32">
-        <v>9.104489218576708</v>
+        <v>8.880892518164108</v>
       </c>
       <c r="F32">
-        <v>3.06917602620251</v>
+        <v>3.232957748931967</v>
       </c>
       <c r="G32">
-        <v>-11.8</v>
+        <v>-12.8</v>
       </c>
       <c r="H32">
-        <v>0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2019 - (sep 2023 - aug 2025)</t>
+          <t>2019 - (aug 2023 - jul 2025)</t>
         </is>
       </c>
       <c r="J32" s="2">
-        <v>45870</v>
+        <v>45839</v>
       </c>
       <c r="K32">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L32">
         <v>2025</v>
@@ -8005,44 +8020,134 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>0.9484594993530926</v>
+        <v>0.9424201687562938</v>
       </c>
       <c r="B33">
-        <v>-5.154050064690741</v>
+        <v>-5.757983124370625</v>
       </c>
       <c r="C33">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D33">
-        <v>9.461194469994499</v>
+        <v>8.761728922821021</v>
       </c>
       <c r="E33">
-        <v>9.229410045651292</v>
+        <v>9.104489218576708</v>
       </c>
       <c r="F33">
-        <v>3.0015883470018</v>
+        <v>3.06917602620251</v>
       </c>
       <c r="G33">
-        <v>-11</v>
+        <v>-11.8</v>
       </c>
       <c r="H33">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2019 - (okt 2023 - sep 2025)</t>
+          <t>2019 - (sep 2023 - aug 2025)</t>
         </is>
       </c>
       <c r="J33" s="2">
-        <v>45901</v>
+        <v>45870</v>
       </c>
       <c r="K33">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L33">
         <v>2025</v>
       </c>
       <c r="M33" t="inlineStr">
+        <is>
+          <t>24_months</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>0.9484594993530926</v>
+      </c>
+      <c r="B34">
+        <v>-5.154050064690741</v>
+      </c>
+      <c r="C34">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>9.461194469994499</v>
+      </c>
+      <c r="E34">
+        <v>9.229410045651292</v>
+      </c>
+      <c r="F34">
+        <v>3.0015883470018</v>
+      </c>
+      <c r="G34">
+        <v>-11</v>
+      </c>
+      <c r="H34">
+        <v>0.7</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2019 - (okt 2023 - sep 2025)</t>
+        </is>
+      </c>
+      <c r="J34" s="2">
+        <v>45901</v>
+      </c>
+      <c r="K34">
+        <v>9</v>
+      </c>
+      <c r="L34">
+        <v>2025</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>24_months</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>0.9504647415344348</v>
+      </c>
+      <c r="B35">
+        <v>-4.953525846556516</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>9.461194469994499</v>
+      </c>
+      <c r="E35">
+        <v>9.445356864131334</v>
+      </c>
+      <c r="F35">
+        <v>3.066579836549348</v>
+      </c>
+      <c r="G35">
+        <v>-11</v>
+      </c>
+      <c r="H35">
+        <v>1.1</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2019 - (nov 2023 - okt 2025)</t>
+        </is>
+      </c>
+      <c r="J35" s="2">
+        <v>45931</v>
+      </c>
+      <c r="K35">
+        <v>10</v>
+      </c>
+      <c r="L35">
+        <v>2025</v>
+      </c>
+      <c r="M35" t="inlineStr">
         <is>
           <t>24_months</t>
         </is>

</xml_diff>

<commit_message>
City index 25-11 6/12 WIP
</commit_message>
<xml_diff>
--- a/data_indexpoints_tidy/tallmateriale_16952.xlsx
+++ b/data_indexpoints_tidy/tallmateriale_16952.xlsx
@@ -2452,10 +2452,10 @@
         <v>2024</v>
       </c>
       <c r="P31">
-        <v>4060</v>
+        <v>10070</v>
       </c>
       <c r="Q31">
-        <v>810</v>
+        <v>1420</v>
       </c>
     </row>
   </sheetData>
@@ -2981,6 +2981,9 @@
       <c r="N13">
         <v>1.78</v>
       </c>
+      <c r="O13">
+        <v>-1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3143,6 +3146,9 @@
       <c r="N16">
         <v>3.49</v>
       </c>
+      <c r="O16">
+        <v>0.47</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3305,6 +3311,9 @@
       <c r="N19">
         <v>5.67</v>
       </c>
+      <c r="O19">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3593,6 +3602,9 @@
       <c r="N25">
         <v>-2.89</v>
       </c>
+      <c r="O25">
+        <v>-8.73</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3974,6 +3986,9 @@
       <c r="N34">
         <v>5.88</v>
       </c>
+      <c r="O34">
+        <v>2.17</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4259,6 +4274,9 @@
       <c r="N40">
         <v>2.24</v>
       </c>
+      <c r="O40">
+        <v>-0.24</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4676,6 +4694,9 @@
       <c r="N49">
         <v>2.43</v>
       </c>
+      <c r="O49">
+        <v>-0.45</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5102,6 +5123,9 @@
       <c r="N58">
         <v>-4.11</v>
       </c>
+      <c r="O58">
+        <v>-7.43</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5264,6 +5288,9 @@
       <c r="N61">
         <v>7.25</v>
       </c>
+      <c r="O61">
+        <v>6.39</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5420,6 +5447,9 @@
       <c r="N64">
         <v>2.87</v>
       </c>
+      <c r="O64">
+        <v>0.54</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5732,6 +5762,9 @@
       <c r="N73">
         <v>-0.33</v>
       </c>
+      <c r="O73">
+        <v>-5.31</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -5861,6 +5894,9 @@
       <c r="N76">
         <v>9.93</v>
       </c>
+      <c r="O76">
+        <v>9.630000000000001</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -5989,6 +6025,9 @@
       </c>
       <c r="N79">
         <v>8.1</v>
+      </c>
+      <c r="O79">
+        <v>8.83</v>
       </c>
     </row>
     <row r="80">
@@ -6358,7 +6397,7 @@
         <v>2025</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -6372,26 +6411,26 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>jan-okt</t>
+          <t>jan-nov</t>
         </is>
       </c>
       <c r="G5">
         <v>18</v>
       </c>
       <c r="H5">
-        <v>1.014</v>
+        <v>1.0127</v>
       </c>
       <c r="I5">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="J5">
-        <v>1.116766126251205</v>
+        <v>1.141741421857783</v>
       </c>
       <c r="K5">
-        <v>-0.8</v>
+        <v>-0.9</v>
       </c>
       <c r="L5">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -6547,7 +6586,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7660,55 +7699,55 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>0.9407166855002579</v>
+        <v>0.956676435683516</v>
       </c>
       <c r="B25">
-        <v>-5.928331449974211</v>
+        <v>-4.332356431648399</v>
       </c>
       <c r="C25">
         <v>14</v>
       </c>
       <c r="D25">
-        <v>9.85146347193337</v>
+        <v>9.461194469994499</v>
       </c>
       <c r="E25">
-        <v>7.329273390694706</v>
+        <v>10.84107229899311</v>
       </c>
       <c r="F25">
-        <v>2.395542921504799</v>
+        <v>3.487192733000519</v>
       </c>
       <c r="G25">
-        <v>-10.6</v>
+        <v>-11.2</v>
       </c>
       <c r="H25">
-        <v>-1.2</v>
+        <v>2.5</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2019 - (jan 2023 - des 2024)</t>
+          <t>2019 - (des 2024 - nov 2025)</t>
         </is>
       </c>
       <c r="J25" s="2">
-        <v>45627</v>
+        <v>45962</v>
       </c>
       <c r="K25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L25">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>24_months</t>
+          <t>12_months</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>0.9448885225160316</v>
+        <v>0.9407166855002579</v>
       </c>
       <c r="B26">
-        <v>-5.511147748396839</v>
+        <v>-5.928331449974211</v>
       </c>
       <c r="C26">
         <v>14</v>
@@ -7717,30 +7756,30 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E26">
-        <v>7.751253966998971</v>
+        <v>7.329273390694706</v>
       </c>
       <c r="F26">
-        <v>2.5175465032293</v>
+        <v>2.395542921504799</v>
       </c>
       <c r="G26">
-        <v>-10.4</v>
+        <v>-10.6</v>
       </c>
       <c r="H26">
-        <v>-0.6</v>
+        <v>-1.2</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2019 - (feb 2023 - jan 2025)</t>
+          <t>2019 - (jan 2023 - des 2024)</t>
         </is>
       </c>
       <c r="J26" s="2">
-        <v>45658</v>
+        <v>45627</v>
       </c>
       <c r="K26">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L26">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="M26" t="inlineStr">
         <is>
@@ -7750,10 +7789,10 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>0.9493633079377803</v>
+        <v>0.9448885225160316</v>
       </c>
       <c r="B27">
-        <v>-5.063669206221966</v>
+        <v>-5.511147748396839</v>
       </c>
       <c r="C27">
         <v>14</v>
@@ -7762,27 +7801,27 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E27">
-        <v>8.199525507506396</v>
+        <v>7.751253966998971</v>
       </c>
       <c r="F27">
-        <v>2.647875692112421</v>
+        <v>2.5175465032293</v>
       </c>
       <c r="G27">
-        <v>-10.3</v>
+        <v>-10.4</v>
       </c>
       <c r="H27">
-        <v>0.1</v>
+        <v>-0.6</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2019 - (mar 2023 - feb 2025)</t>
+          <t>2019 - (feb 2023 - jan 2025)</t>
         </is>
       </c>
       <c r="J27" s="2">
-        <v>45689</v>
+        <v>45658</v>
       </c>
       <c r="K27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L27">
         <v>2025</v>
@@ -7795,10 +7834,10 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>0.9501717700140583</v>
+        <v>0.9493633079377803</v>
       </c>
       <c r="B28">
-        <v>-4.982822998594171</v>
+        <v>-5.063669206221966</v>
       </c>
       <c r="C28">
         <v>14</v>
@@ -7807,27 +7846,27 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E28">
-        <v>8.616161112309243</v>
+        <v>8.199525507506396</v>
       </c>
       <c r="F28">
-        <v>2.768619629046594</v>
+        <v>2.647875692112421</v>
       </c>
       <c r="G28">
-        <v>-10.4</v>
+        <v>-10.3</v>
       </c>
       <c r="H28">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2019 - (apr 2023 - mar 2025)</t>
+          <t>2019 - (mar 2023 - feb 2025)</t>
         </is>
       </c>
       <c r="J28" s="2">
-        <v>45717</v>
+        <v>45689</v>
       </c>
       <c r="K28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L28">
         <v>2025</v>
@@ -7840,10 +7879,10 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>0.9538765915536376</v>
+        <v>0.9501717700140583</v>
       </c>
       <c r="B29">
-        <v>-4.612340844636242</v>
+        <v>-4.982822998594171</v>
       </c>
       <c r="C29">
         <v>14</v>
@@ -7852,27 +7891,27 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E29">
-        <v>9.190469092064667</v>
+        <v>8.616161112309243</v>
       </c>
       <c r="F29">
-        <v>2.936645120593631</v>
+        <v>2.768619629046594</v>
       </c>
       <c r="G29">
         <v>-10.4</v>
       </c>
       <c r="H29">
-        <v>1.1</v>
+        <v>0.4</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2019 - (mai 2023 - apr 2025)</t>
+          <t>2019 - (apr 2023 - mar 2025)</t>
         </is>
       </c>
       <c r="J29" s="2">
-        <v>45748</v>
+        <v>45717</v>
       </c>
       <c r="K29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L29">
         <v>2025</v>
@@ -7885,10 +7924,10 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>0.9566542182687537</v>
+        <v>0.9538765915536376</v>
       </c>
       <c r="B30">
-        <v>-4.334578173124626</v>
+        <v>-4.612340844636242</v>
       </c>
       <c r="C30">
         <v>14</v>
@@ -7897,27 +7936,27 @@
         <v>9.85146347193337</v>
       </c>
       <c r="E30">
-        <v>9.660527652721862</v>
+        <v>9.190469092064667</v>
       </c>
       <c r="F30">
-        <v>3.074711764079583</v>
+        <v>2.936645120593631</v>
       </c>
       <c r="G30">
         <v>-10.4</v>
       </c>
       <c r="H30">
-        <v>1.7</v>
+        <v>1.1</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2019 - (jun 2023 - mai 2025)</t>
+          <t>2019 - (mai 2023 - apr 2025)</t>
         </is>
       </c>
       <c r="J30" s="2">
-        <v>45778</v>
+        <v>45748</v>
       </c>
       <c r="K30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L30">
         <v>2025</v>
@@ -7930,39 +7969,39 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>0.9337995597988019</v>
+        <v>0.9566542182687537</v>
       </c>
       <c r="B31">
-        <v>-6.620044020119808</v>
+        <v>-4.334578173124626</v>
       </c>
       <c r="C31">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D31">
-        <v>8.176539225649242</v>
+        <v>9.85146347193337</v>
       </c>
       <c r="E31">
-        <v>7.9106263041602</v>
+        <v>9.660527652721862</v>
       </c>
       <c r="F31">
-        <v>2.783454672675907</v>
+        <v>3.074711764079583</v>
       </c>
       <c r="G31">
-        <v>-12.1</v>
+        <v>-10.4</v>
       </c>
       <c r="H31">
-        <v>-1.2</v>
+        <v>1.7</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2019 - (jul 2023 - jun 2025)</t>
+          <t>2019 - (jun 2023 - mai 2025)</t>
         </is>
       </c>
       <c r="J31" s="2">
-        <v>45809</v>
+        <v>45778</v>
       </c>
       <c r="K31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L31">
         <v>2025</v>
@@ -7975,39 +8014,39 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>0.9355678479216543</v>
+        <v>0.9337995597988019</v>
       </c>
       <c r="B32">
-        <v>-6.443215207834574</v>
+        <v>-6.620044020119808</v>
       </c>
       <c r="C32">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D32">
-        <v>7.442799395296631</v>
+        <v>8.176539225649242</v>
       </c>
       <c r="E32">
-        <v>8.880892518164108</v>
+        <v>7.9106263041602</v>
       </c>
       <c r="F32">
-        <v>3.232957748931967</v>
+        <v>2.783454672675907</v>
       </c>
       <c r="G32">
-        <v>-12.8</v>
+        <v>-12.1</v>
       </c>
       <c r="H32">
-        <v>-0.1</v>
+        <v>-1.2</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2019 - (aug 2023 - jul 2025)</t>
+          <t>2019 - (jul 2023 - jun 2025)</t>
         </is>
       </c>
       <c r="J32" s="2">
-        <v>45839</v>
+        <v>45809</v>
       </c>
       <c r="K32">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L32">
         <v>2025</v>
@@ -8020,39 +8059,39 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>0.9424201687562938</v>
+        <v>0.9355678479216543</v>
       </c>
       <c r="B33">
-        <v>-5.757983124370625</v>
+        <v>-6.443215207834574</v>
       </c>
       <c r="C33">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D33">
-        <v>8.761728922821021</v>
+        <v>7.442799395296631</v>
       </c>
       <c r="E33">
-        <v>9.104489218576708</v>
+        <v>8.880892518164108</v>
       </c>
       <c r="F33">
-        <v>3.06917602620251</v>
+        <v>3.232957748931967</v>
       </c>
       <c r="G33">
-        <v>-11.8</v>
+        <v>-12.8</v>
       </c>
       <c r="H33">
-        <v>0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2019 - (sep 2023 - aug 2025)</t>
+          <t>2019 - (aug 2023 - jul 2025)</t>
         </is>
       </c>
       <c r="J33" s="2">
-        <v>45870</v>
+        <v>45839</v>
       </c>
       <c r="K33">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L33">
         <v>2025</v>
@@ -8065,39 +8104,39 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>0.9484594993530926</v>
+        <v>0.9424201687562938</v>
       </c>
       <c r="B34">
-        <v>-5.154050064690741</v>
+        <v>-5.757983124370625</v>
       </c>
       <c r="C34">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D34">
-        <v>9.461194469994499</v>
+        <v>8.761728922821021</v>
       </c>
       <c r="E34">
-        <v>9.229410045651292</v>
+        <v>9.104489218576708</v>
       </c>
       <c r="F34">
-        <v>3.0015883470018</v>
+        <v>3.06917602620251</v>
       </c>
       <c r="G34">
-        <v>-11</v>
+        <v>-11.8</v>
       </c>
       <c r="H34">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2019 - (okt 2023 - sep 2025)</t>
+          <t>2019 - (sep 2023 - aug 2025)</t>
         </is>
       </c>
       <c r="J34" s="2">
-        <v>45901</v>
+        <v>45870</v>
       </c>
       <c r="K34">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L34">
         <v>2025</v>
@@ -8110,10 +8149,10 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>0.9504647415344348</v>
+        <v>0.9484594993530926</v>
       </c>
       <c r="B35">
-        <v>-4.953525846556516</v>
+        <v>-5.154050064690741</v>
       </c>
       <c r="C35">
         <v>14</v>
@@ -8122,32 +8161,122 @@
         <v>9.461194469994499</v>
       </c>
       <c r="E35">
-        <v>9.445356864131334</v>
+        <v>9.229410045651292</v>
       </c>
       <c r="F35">
-        <v>3.066579836549348</v>
+        <v>3.0015883470018</v>
       </c>
       <c r="G35">
         <v>-11</v>
       </c>
       <c r="H35">
-        <v>1.1</v>
+        <v>0.7</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2019 - (nov 2023 - okt 2025)</t>
+          <t>2019 - (okt 2023 - sep 2025)</t>
         </is>
       </c>
       <c r="J35" s="2">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="K35">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L35">
         <v>2025</v>
       </c>
       <c r="M35" t="inlineStr">
+        <is>
+          <t>24_months</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>0.9504647415344348</v>
+      </c>
+      <c r="B36">
+        <v>-4.953525846556516</v>
+      </c>
+      <c r="C36">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>9.461194469994499</v>
+      </c>
+      <c r="E36">
+        <v>9.445356864131334</v>
+      </c>
+      <c r="F36">
+        <v>3.066579836549348</v>
+      </c>
+      <c r="G36">
+        <v>-11</v>
+      </c>
+      <c r="H36">
+        <v>1.1</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2019 - (nov 2023 - okt 2025)</t>
+        </is>
+      </c>
+      <c r="J36" s="2">
+        <v>45931</v>
+      </c>
+      <c r="K36">
+        <v>10</v>
+      </c>
+      <c r="L36">
+        <v>2025</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>24_months</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>0.9505415319810241</v>
+      </c>
+      <c r="B37">
+        <v>-4.945846801897591</v>
+      </c>
+      <c r="C37">
+        <v>14</v>
+      </c>
+      <c r="D37">
+        <v>9.461194469994499</v>
+      </c>
+      <c r="E37">
+        <v>9.649200500987547</v>
+      </c>
+      <c r="F37">
+        <v>3.1275596420733</v>
+      </c>
+      <c r="G37">
+        <v>-11.1</v>
+      </c>
+      <c r="H37">
+        <v>1.2</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2019 - (des 2023 - nov 2025)</t>
+        </is>
+      </c>
+      <c r="J37" s="2">
+        <v>45962</v>
+      </c>
+      <c r="K37">
+        <v>11</v>
+      </c>
+      <c r="L37">
+        <v>2025</v>
+      </c>
+      <c r="M37" t="inlineStr">
         <is>
           <t>24_months</t>
         </is>

</xml_diff>